<commit_message>
more graphs, style changes
</commit_message>
<xml_diff>
--- a/hackSMU/hackSMUII/check_ins.xlsx
+++ b/hackSMU/hackSMUII/check_ins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\n-wes\Github\Data-Visualization-with-Python\hackSMU\hackSMUII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA17E73-3D78-42DD-914A-763ECEE3D9AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EBFEAC-BFB7-48C4-89D4-A27D5A3583AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="110">
   <si>
     <t>Timestamp</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Sridhar Nandigam</t>
   </si>
   <si>
-    <t xml:space="preserve">University of North Texas </t>
-  </si>
-  <si>
     <t>Software Engineering, Data Science, Entrepreneurship and "The Business Side"</t>
   </si>
   <si>
@@ -124,15 +121,9 @@
     <t>Dinesh Polisetty</t>
   </si>
   <si>
-    <t>Centenniel High School</t>
-  </si>
-  <si>
     <t>Abhinav Kolli</t>
   </si>
   <si>
-    <t>Centennial High school</t>
-  </si>
-  <si>
     <t>Jonas Moros</t>
   </si>
   <si>
@@ -355,10 +346,10 @@
     <t>Registered</t>
   </si>
   <si>
-    <t xml:space="preserve">Southern Methodist University </t>
-  </si>
-  <si>
     <t>TAMS</t>
+  </si>
+  <si>
+    <t>Centennial High School</t>
   </si>
 </sst>
 </file>
@@ -627,7 +618,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -652,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -697,7 +688,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -731,10 +722,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>7</v>
@@ -745,13 +736,13 @@
         <v>43862.462165810182</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>7</v>
@@ -762,10 +753,10 @@
         <v>43862.462213599538</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
@@ -779,13 +770,13 @@
         <v>43862.464893680561</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
@@ -796,13 +787,13 @@
         <v>43862.466029143514</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>7</v>
@@ -813,10 +804,10 @@
         <v>43862.466103356477</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>13</v>
@@ -830,13 +821,13 @@
         <v>43862.466133124995</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -847,7 +838,7 @@
         <v>43862.466463495366</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -864,10 +855,10 @@
         <v>43862.466529594909</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
@@ -881,13 +872,13 @@
         <v>43862.467366805555</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>7</v>
@@ -898,10 +889,10 @@
         <v>43862.467369861115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>6</v>
@@ -915,10 +906,10 @@
         <v>43862.467598773146</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>6</v>
@@ -932,13 +923,13 @@
         <v>43862.472858437497</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
@@ -949,13 +940,13 @@
         <v>43862.474299444446</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
@@ -966,13 +957,13 @@
         <v>43862.474456851851</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
@@ -983,10 +974,10 @@
         <v>43862.47489863426</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>13</v>
@@ -1000,13 +991,13 @@
         <v>43862.476663668982</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
@@ -1017,7 +1008,7 @@
         <v>43862.476919583336</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
@@ -1034,13 +1025,13 @@
         <v>43862.476965277776</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>11</v>
@@ -1051,7 +1042,7 @@
         <v>43862.481148032406</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
@@ -1068,13 +1059,13 @@
         <v>43862.482102013892</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>7</v>
@@ -1085,13 +1076,13 @@
         <v>43862.482808483794</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>7</v>
@@ -1102,13 +1093,13 @@
         <v>43862.486695729167</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>7</v>
@@ -1119,7 +1110,7 @@
         <v>43862.489596388885</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
@@ -1136,13 +1127,13 @@
         <v>43862.492689502316</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>7</v>
@@ -1153,13 +1144,13 @@
         <v>43862.496939236109</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>7</v>
@@ -1170,13 +1161,13 @@
         <v>43862.506009189819</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>7</v>
@@ -1187,7 +1178,7 @@
         <v>43862.506126840279</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>9</v>
@@ -1204,13 +1195,13 @@
         <v>43862.50632612269</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>7</v>
@@ -1221,13 +1212,13 @@
         <v>43862.508575914355</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
@@ -1238,13 +1229,13 @@
         <v>43862.515477870373</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>11</v>
@@ -1255,13 +1246,13 @@
         <v>43862.543520185187</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>11</v>
@@ -1272,7 +1263,7 @@
         <v>43862.547404340279</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>9</v>
@@ -1289,13 +1280,13 @@
         <v>43862.551328865738</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>11</v>
@@ -1306,13 +1297,13 @@
         <v>43862.551350729162</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>11</v>
@@ -1323,13 +1314,13 @@
         <v>43862.551730312502</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>11</v>
@@ -1340,13 +1331,13 @@
         <v>43862.551808888893</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>11</v>
@@ -1357,7 +1348,7 @@
         <v>43862.553126608793</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>9</v>
@@ -1374,7 +1365,7 @@
         <v>43862.553600115745</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>9</v>
@@ -1391,7 +1382,7 @@
         <v>43862.553820671295</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>9</v>
@@ -1408,7 +1399,7 @@
         <v>43862.55407622685</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>9</v>
@@ -1425,13 +1416,13 @@
         <v>43862.554509074078</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>7</v>
@@ -1442,13 +1433,13 @@
         <v>43862.561076388884</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>11</v>
@@ -1459,13 +1450,13 @@
         <v>43862.561401157407</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>11</v>
@@ -1476,7 +1467,7 @@
         <v>43862.566036273143</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>9</v>
@@ -1493,13 +1484,13 @@
         <v>43862.57132181713</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>11</v>
@@ -1510,7 +1501,7 @@
         <v>43862.576851122685</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>9</v>
@@ -1527,13 +1518,13 @@
         <v>43862.596346099541</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>11</v>
@@ -1544,13 +1535,13 @@
         <v>43862.606878923616</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>7</v>
@@ -1561,13 +1552,13 @@
         <v>43862.62620481482</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>7</v>
@@ -1578,13 +1569,13 @@
         <v>43862.626295289352</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>7</v>
@@ -1595,13 +1586,13 @@
         <v>43862.653911400463</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>11</v>
@@ -1612,13 +1603,13 @@
         <v>43862.654198379634</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>11</v>
@@ -1629,13 +1620,13 @@
         <v>43862.688832812499</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>7</v>
@@ -1646,13 +1637,13 @@
         <v>43862.690636643514</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>7</v>
@@ -1663,7 +1654,7 @@
         <v>43862.801325335648</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>9</v>
@@ -1677,7 +1668,7 @@
         <v>43862.825954432876</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>9</v>
@@ -1694,13 +1685,13 @@
         <v>43862.82668784722</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>11</v>
@@ -1711,13 +1702,13 @@
         <v>43862.867463935181</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>11</v>
@@ -1728,13 +1719,13 @@
         <v>43862.868302962961</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>11</v>
@@ -1745,13 +1736,13 @@
         <v>43863.451362997686</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>11</v>
@@ -1762,13 +1753,13 @@
         <v>43863.474886354168</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>11</v>
@@ -1779,13 +1770,13 @@
         <v>43863.482690752317</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>7</v>
@@ -1796,13 +1787,13 @@
         <v>43863.488039606484</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>11</v>
@@ -1813,13 +1804,13 @@
         <v>43863.48828336806</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>11</v>
@@ -1830,13 +1821,13 @@
         <v>43863.534182766205</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>11</v>
@@ -1847,13 +1838,13 @@
         <v>43863.534640081023</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>11</v>

</xml_diff>